<commit_message>
debugging execution crash at t=0.3secs
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/MiniBanshee/relay_settings/F3_relay_banshee.xlsx
+++ b/DistributionSystems/SimulinkOpal/MiniBanshee/relay_settings/F3_relay_banshee.xlsx
@@ -209,7 +209,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6225872" cy="4914679"/>
@@ -773,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +892,7 @@
         <v>600</v>
       </c>
       <c r="H2" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="6">
         <v>20</v>
@@ -957,10 +957,10 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="6">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H3" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
         <v>20</v>
@@ -1025,7 +1025,7 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="6">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -1074,415 +1074,73 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>13800</v>
-      </c>
-      <c r="C5" s="5">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="6">
-        <v>600</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6">
-        <v>20</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="L5" s="6">
-        <v>1</v>
-      </c>
-      <c r="M5" s="6">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="O5" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P5" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>1</v>
-      </c>
-      <c r="R5" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="S5" s="6">
-        <v>2</v>
-      </c>
-      <c r="T5" s="6">
-        <v>3</v>
-      </c>
-      <c r="U5" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="V5" s="6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A5" s="12"/>
+      <c r="B5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
-        <v>13800</v>
-      </c>
-      <c r="C6" s="5">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="6">
-        <v>200</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>20</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="L6" s="6">
-        <v>1</v>
-      </c>
-      <c r="M6" s="6">
-        <v>1</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="O6" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P6" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="S6" s="6">
-        <v>2</v>
-      </c>
-      <c r="T6" s="6">
-        <v>3</v>
-      </c>
-      <c r="U6" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="V6" s="6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>13800</v>
-      </c>
-      <c r="C7" s="5">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="6">
-        <v>200</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>20</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="L7" s="6">
-        <v>1</v>
-      </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="O7" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P7" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>1</v>
-      </c>
-      <c r="R7" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="S7" s="6">
-        <v>2</v>
-      </c>
-      <c r="T7" s="6">
-        <v>3</v>
-      </c>
-      <c r="U7" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="V7" s="6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>480</v>
-      </c>
-      <c r="C8" s="5">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1500</v>
-      </c>
-      <c r="H8" s="11">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6">
-        <v>20</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P8" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>1</v>
-      </c>
-      <c r="R8" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="S8" s="6">
-        <v>2</v>
-      </c>
-      <c r="T8" s="6">
-        <v>3</v>
-      </c>
-      <c r="U8" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="V8" s="6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6">
-        <v>480</v>
-      </c>
-      <c r="C9" s="5">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1500</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>20</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="L9" s="6">
-        <v>1</v>
-      </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="O9" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P9" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>1</v>
-      </c>
-      <c r="R9" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="S9" s="6">
-        <v>2</v>
-      </c>
-      <c r="T9" s="6">
-        <v>3</v>
-      </c>
-      <c r="U9" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="V9" s="6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>480</v>
-      </c>
-      <c r="C10" s="5">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="6">
-        <v>2200</v>
-      </c>
-      <c r="H10" s="11">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>20</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="L10" s="6">
-        <v>1</v>
-      </c>
-      <c r="M10" s="6">
-        <v>1</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="O10" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P10" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>1</v>
-      </c>
-      <c r="R10" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="S10" s="6">
-        <v>2</v>
-      </c>
-      <c r="T10" s="6">
-        <v>3</v>
-      </c>
-      <c r="U10" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="V10" s="6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1514,72 +1172,6 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>